<commit_message>
Rename arc to link
</commit_message>
<xml_diff>
--- a/examples/max-flow.xlsx
+++ b/examples/max-flow.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="2" r:id="rId1"/>
-    <sheet name="arcs" sheetId="1" r:id="rId2"/>
+    <sheet name="links" sheetId="1" r:id="rId2"/>
     <sheet name="scale" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -431,12 +431,12 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -450,7 +450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -478,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -492,7 +492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -533,14 +533,14 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -560,7 +560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -580,7 +580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -680,21 +680,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -715,17 +715,17 @@
       <selection activeCell="C9" sqref="C9:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -733,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -741,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -749,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -757,7 +757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -765,12 +765,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -786,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -794,7 +794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -802,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>

</xml_diff>